<commit_message>
Yield Curve Decomposition - Full Repricing
</commit_message>
<xml_diff>
--- a/Fixed Income Attribution.xlsx
+++ b/Fixed Income Attribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kc111\Dev\CIPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B97DA3E-E4A1-4A78-BC9F-7ADB770689DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5512610-856A-4804-9DC8-49F2038A8336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{A0219E52-BC5C-483A-9CFD-680264FDC4D2}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
   <si>
     <t>Bond</t>
   </si>
@@ -208,6 +208,72 @@
   </si>
   <si>
     <t>Added Value</t>
+  </si>
+  <si>
+    <t>Yield Curve Decomposition - Full Repricing</t>
+  </si>
+  <si>
+    <t>Spot Rate</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>6/30/132</t>
+  </si>
+  <si>
+    <t>Amortized</t>
+  </si>
+  <si>
+    <t>Sloped</t>
+  </si>
+  <si>
+    <t>Shifted</t>
+  </si>
+  <si>
+    <t>Systematic</t>
+  </si>
+  <si>
+    <t>Price Return</t>
+  </si>
+  <si>
+    <t>Coupon Return</t>
+  </si>
+  <si>
+    <t>Total Return</t>
+  </si>
+  <si>
+    <t>Passage of time</t>
+  </si>
+  <si>
+    <t>Amortization</t>
+  </si>
+  <si>
+    <t>Roll down</t>
+  </si>
+  <si>
+    <t>Curve variation</t>
+  </si>
+  <si>
+    <t>Spread variations</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Exhibit 66: Single Bond Return Attribution</t>
+  </si>
+  <si>
+    <t>Begin (T)</t>
+  </si>
+  <si>
+    <t>End (T+1)</t>
+  </si>
+  <si>
+    <t>Systmatic spread</t>
+  </si>
+  <si>
+    <t>Exhibit 65: Summary of Price Return Factors</t>
   </si>
 </sst>
 </file>
@@ -264,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +346,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -388,6 +460,19 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -726,13 +811,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F012BF49-FE1B-4160-A766-CE0F833F361B}">
-  <dimension ref="A1:CA17"/>
+  <dimension ref="A1:CW18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="AD7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="BF7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AY15" sqref="AY15"/>
+      <selection pane="bottomRight" activeCell="CC1" sqref="CC1:CW1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -806,10 +891,24 @@
     <col min="77" max="77" width="7.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="80" max="16384" width="8.88671875" style="1"/>
+    <col min="80" max="80" width="8.88671875" style="1"/>
+    <col min="81" max="81" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="8.88671875" style="1" customWidth="1"/>
+    <col min="85" max="85" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="6.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8.88671875" style="1"/>
+    <col min="92" max="92" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="6.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="94" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>35</v>
       </c>
@@ -892,8 +991,31 @@
       <c r="BY1" s="29"/>
       <c r="BZ1" s="29"/>
       <c r="CA1" s="29"/>
+      <c r="CC1" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="CD1" s="29"/>
+      <c r="CE1" s="29"/>
+      <c r="CF1" s="29"/>
+      <c r="CG1" s="29"/>
+      <c r="CH1" s="29"/>
+      <c r="CI1" s="29"/>
+      <c r="CJ1" s="29"/>
+      <c r="CK1" s="29"/>
+      <c r="CL1" s="29"/>
+      <c r="CM1" s="29"/>
+      <c r="CN1" s="29"/>
+      <c r="CO1" s="29"/>
+      <c r="CP1" s="29"/>
+      <c r="CQ1" s="29"/>
+      <c r="CR1" s="29"/>
+      <c r="CS1" s="29"/>
+      <c r="CT1" s="29"/>
+      <c r="CU1" s="29"/>
+      <c r="CV1" s="29"/>
+      <c r="CW1" s="29"/>
     </row>
-    <row r="2" spans="1:79" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38"/>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -972,8 +1094,10 @@
       <c r="BY2" s="30"/>
       <c r="BZ2" s="30"/>
       <c r="CA2" s="30"/>
+      <c r="CL2" s="31"/>
+      <c r="CO2" s="31"/>
     </row>
-    <row r="3" spans="1:79" s="35" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" s="35" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>1</v>
       </c>
@@ -1062,8 +1186,25 @@
       <c r="BY3" s="34"/>
       <c r="BZ3" s="34"/>
       <c r="CA3" s="34"/>
+      <c r="CC3" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="CD3" s="34"/>
+      <c r="CE3" s="34"/>
+      <c r="CF3" s="34"/>
+      <c r="CG3" s="34"/>
+      <c r="CH3" s="34"/>
+      <c r="CJ3" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="CK3" s="45"/>
+      <c r="CL3" s="45"/>
+      <c r="CN3" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="CO3" s="45"/>
     </row>
-    <row r="4" spans="1:79" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:101" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -1084,8 +1225,13 @@
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
+      <c r="CJ4" s="45"/>
+      <c r="CK4" s="45"/>
+      <c r="CL4" s="45"/>
+      <c r="CN4" s="45"/>
+      <c r="CO4" s="45"/>
     </row>
-    <row r="5" spans="1:79" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:101" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I5" s="4">
         <v>41455</v>
       </c>
@@ -1174,8 +1320,18 @@
       <c r="BY5" s="3"/>
       <c r="BZ5" s="3"/>
       <c r="CA5" s="3"/>
+      <c r="CD5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="CE5" s="3"/>
+      <c r="CF5" s="3"/>
+      <c r="CG5" s="3"/>
+      <c r="CH5" s="3"/>
+      <c r="CI5" s="5"/>
+      <c r="CL5" s="40"/>
+      <c r="CO5" s="40"/>
     </row>
-    <row r="6" spans="1:79" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:101" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1391,8 +1547,34 @@
       <c r="CA6" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="CC6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="CD6" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="CE6" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="CF6" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="CG6" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="CH6" s="39">
+        <v>41639</v>
+      </c>
+      <c r="CJ6" s="39"/>
+      <c r="CK6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="CL6" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="CO6" s="40"/>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str" cm="1">
         <f t="array" ref="A7:A13">B7:B13&amp;" "&amp;TEXT(C7:C13,"0%")&amp;" "&amp;TEXT(D7:D13,"DD MMM YYYY")</f>
         <v>Government 5% 30 Jun 2018</v>
@@ -1407,8 +1589,8 @@
         <v>43281</v>
       </c>
       <c r="E7" s="13" cm="1">
-        <f t="array" ref="E7:E13">(D7:D13-I5)/365</f>
-        <v>5.0027397260273974</v>
+        <f t="array" ref="E7:E13">ROUND((D7:D13-I5)/365,0)</f>
+        <v>5</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>23</v>
@@ -1640,8 +1822,40 @@
       <c r="CA7" s="17">
         <v>3.4786729857819972E-3</v>
       </c>
+      <c r="CC7" s="1">
+        <v>1</v>
+      </c>
+      <c r="CD7" s="15">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="CE7" s="32">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="CF7" s="32">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="CG7" s="32">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="CH7" s="32">
+        <v>3.85E-2</v>
+      </c>
+      <c r="CJ7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="CK7" s="18" cm="1">
+        <f t="array" ref="CK7">SUM((_xlfn.FLOOR.MATH(_xlfn.SEQUENCE($E$10*2)/($E$10*2))*100+$M$10*100)*(1+$CD$7:$CD$16/2)^-$CC$7:$CC$16)</f>
+        <v>103.19974147561445</v>
+      </c>
+      <c r="CN7" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="CO7" s="44">
+        <f>SUM(CO8:CO10)</f>
+        <v>2.5171632906759854E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="str">
         <v>Government 7% 30 Jun 2023</v>
       </c>
@@ -1655,7 +1869,7 @@
         <v>45107</v>
       </c>
       <c r="E8" s="13">
-        <v>10.005479452054795</v>
+        <v>10</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>24</v>
@@ -1870,8 +2084,44 @@
       <c r="CA8" s="17">
         <v>5.1603330310774119E-3</v>
       </c>
+      <c r="CC8" s="1">
+        <v>2</v>
+      </c>
+      <c r="CD8" s="15">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="CE8" s="32">
+        <v>4.1799999999999997E-2</v>
+      </c>
+      <c r="CF8" s="32">
+        <v>4.2130000000000001E-2</v>
+      </c>
+      <c r="CG8" s="32">
+        <v>4.4130000000000003E-2</v>
+      </c>
+      <c r="CH8" s="32">
+        <v>4.5100000000000001E-2</v>
+      </c>
+      <c r="CJ8" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="CK8" s="18" cm="1">
+        <f t="array" ref="CK8">SUM((_xlfn.FLOOR.MATH(_xlfn.SEQUENCE($E$10*2-1)/($E$10*2-1))*100+$M$10*100)*(1+$CD$8:$CD$16/2)^-$CC$7:$CC$15)</f>
+        <v>102.85016958158496</v>
+      </c>
+      <c r="CL8" s="17">
+        <f>(CK8-CK7)/CK$7</f>
+        <v>-3.3873330400937367E-3</v>
+      </c>
+      <c r="CN8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="CO8" s="17">
+        <f>CL16</f>
+        <v>2.4224866886810338E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="str">
         <v>Government 6% 30 Jun 2028</v>
       </c>
@@ -1885,7 +2135,7 @@
         <v>46934</v>
       </c>
       <c r="E9" s="13">
-        <v>15.010958904109589</v>
+        <v>15</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>25</v>
@@ -2100,8 +2350,44 @@
       <c r="CA9" s="17">
         <v>-2.1870352550083104E-3</v>
       </c>
+      <c r="CC9" s="1">
+        <v>3</v>
+      </c>
+      <c r="CD9" s="15">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="CE9" s="32">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="CF9" s="32">
+        <v>4.607E-2</v>
+      </c>
+      <c r="CG9" s="32">
+        <v>4.8070000000000002E-2</v>
+      </c>
+      <c r="CH9" s="32">
+        <v>4.9100000000000005E-2</v>
+      </c>
+      <c r="CJ9" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="CK9" s="18" cm="1">
+        <f t="array" ref="CK9">SUM((_xlfn.FLOOR.MATH(_xlfn.SEQUENCE($E$10*2-1)/($E$10*2-1))*100+$M$10*100)*(1+$CD$7:$CD$15/2)^-$CC$7:$CC$15)</f>
+        <v>103.29744748411113</v>
+      </c>
+      <c r="CL9" s="17">
+        <f t="shared" ref="CL9:CL14" si="0">(CK9-CK8)/CK$7</f>
+        <v>4.3340990600432535E-3</v>
+      </c>
+      <c r="CN9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="CO9" s="17" cm="1">
+        <f t="array" ref="CO9:CO10">CL8:CL9</f>
+        <v>-3.3873330400937367E-3</v>
+      </c>
     </row>
-    <row r="10" spans="1:79" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="str">
         <v>Corporate 5% 30 Jun 2018</v>
       </c>
@@ -2115,7 +2401,7 @@
         <v>43281</v>
       </c>
       <c r="E10" s="13">
-        <v>5.0027397260273974</v>
+        <v>5</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>23</v>
@@ -2256,8 +2542,43 @@
       <c r="CA10" s="17">
         <v>2.1656976744186054E-3</v>
       </c>
+      <c r="CC10" s="1">
+        <v>4</v>
+      </c>
+      <c r="CD10" s="15">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="CE10" s="32">
+        <v>4.7899999999999998E-2</v>
+      </c>
+      <c r="CF10" s="32">
+        <v>4.8899999999999999E-2</v>
+      </c>
+      <c r="CG10" s="32">
+        <v>5.0900000000000001E-2</v>
+      </c>
+      <c r="CH10" s="32">
+        <v>5.1900000000000002E-2</v>
+      </c>
+      <c r="CJ10" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="CK10" s="18" cm="1">
+        <f t="array" ref="CK10">SUM((_xlfn.FLOOR.MATH(_xlfn.SEQUENCE($E$10*2-1)/($E$10*2-1))*100+$M$10*100)*(1+($CD$7:$CD$15+0.01)/2)^-$CC$7:$CC$15)</f>
+        <v>99.257256810076242</v>
+      </c>
+      <c r="CL10" s="17">
+        <f t="shared" si="0"/>
+        <v>-3.9149232510331096E-2</v>
+      </c>
+      <c r="CN10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="CO10" s="17">
+        <v>4.3340990600432535E-3</v>
+      </c>
     </row>
-    <row r="11" spans="1:79" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:101" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="str">
         <v>Corporate 7% 30 Jun 2023</v>
       </c>
@@ -2271,7 +2592,7 @@
         <v>45107</v>
       </c>
       <c r="E11" s="13">
-        <v>10.005479452054795</v>
+        <v>10</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>24</v>
@@ -2438,8 +2759,44 @@
       <c r="CA11" s="17">
         <v>-3.0707381746642682E-3</v>
       </c>
+      <c r="CC11" s="1">
+        <v>5</v>
+      </c>
+      <c r="CD11" s="15">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="CE11" s="32">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="CF11" s="32">
+        <v>5.1130000000000002E-2</v>
+      </c>
+      <c r="CG11" s="32">
+        <v>5.3129999999999997E-2</v>
+      </c>
+      <c r="CH11" s="32">
+        <v>5.4100000000000002E-2</v>
+      </c>
+      <c r="CJ11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="CK11" s="18" cm="1">
+        <f t="array" ref="CK11">SUM((_xlfn.FLOOR.MATH(_xlfn.SEQUENCE($E$10*2-1)/($E$10*2-1))*100+$M$10*100)*(1+($CE$7:$CE$15)/2)^-$CC$7:$CC$15)</f>
+        <v>98.368079092837689</v>
+      </c>
+      <c r="CL11" s="17">
+        <f t="shared" si="0"/>
+        <v>-8.616084735528733E-3</v>
+      </c>
+      <c r="CN11" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="CO11" s="44">
+        <f>SUM(_xlfn.ANCHORARRAY(CO12))</f>
+        <v>-5.7386512542221088E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="str">
         <v>Corporate 6% 30 Jun 2028</v>
       </c>
@@ -2453,7 +2810,7 @@
         <v>46934</v>
       </c>
       <c r="E12" s="13">
-        <v>15.010958904109589</v>
+        <v>15</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>25</v>
@@ -2594,8 +2951,44 @@
       <c r="CA12" s="17">
         <v>8.7870148979216373E-3</v>
       </c>
+      <c r="CC12" s="1">
+        <v>6</v>
+      </c>
+      <c r="CD12" s="15">
+        <v>3.85E-2</v>
+      </c>
+      <c r="CE12" s="32">
+        <v>5.1299999999999998E-2</v>
+      </c>
+      <c r="CF12" s="32">
+        <v>5.2970000000000003E-2</v>
+      </c>
+      <c r="CG12" s="32">
+        <v>5.4969999999999998E-2</v>
+      </c>
+      <c r="CH12" s="32">
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="CJ12" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="CK12" s="18" cm="1">
+        <f t="array" ref="CK12">SUM((_xlfn.FLOOR.MATH(_xlfn.SEQUENCE($E$10*2-1)/($E$10*2-1))*100+$M$10*100)*(1+($CF$7:$CF$15)/2)^-$CC$7:$CC$15)</f>
+        <v>97.375174225566809</v>
+      </c>
+      <c r="CL12" s="17">
+        <f t="shared" si="0"/>
+        <v>-9.6211952963612644E-3</v>
+      </c>
+      <c r="CN12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CO12" s="17" cm="1">
+        <f t="array" ref="CO12:CO14">CL10:CL12</f>
+        <v>-3.9149232510331096E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:79" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:101" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="str">
         <v>Corporate 6% 30 Jun 2028</v>
       </c>
@@ -2609,7 +3002,7 @@
         <v>46934</v>
       </c>
       <c r="E13" s="13">
-        <v>15.010958904109589</v>
+        <v>15</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>25</v>
@@ -2780,8 +3173,43 @@
       <c r="CA13" s="17">
         <v>-1.624977009380172E-2</v>
       </c>
+      <c r="CC13" s="1">
+        <v>7</v>
+      </c>
+      <c r="CD13" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="CE13" s="32">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="CF13" s="32">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="CG13" s="32">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="CH13" s="32">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="CJ13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="CK13" s="18" cm="1">
+        <f t="array" ref="CK13">SUM((_xlfn.FLOOR.MATH(_xlfn.SEQUENCE($E$10*2-1)/($E$10*2-1))*100+$M$10*100)*(1+($CG$7:$CG$15)/2)^-$CC$7:$CC$15)</f>
+        <v>96.607434908839338</v>
+      </c>
+      <c r="CL13" s="17">
+        <f t="shared" si="0"/>
+        <v>-7.4393531005974879E-3</v>
+      </c>
+      <c r="CN13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="CO13" s="17">
+        <v>-8.616084735528733E-3</v>
+      </c>
     </row>
-    <row r="14" spans="1:79" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:101" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R14" s="21" cm="1">
         <f t="array" ref="R14:Y14">_xlfn.BYCOL(R7:Y13,_xleta.SUM)</f>
         <v>1</v>
@@ -2902,8 +3330,43 @@
       <c r="CA14" s="31">
         <v>-1.9158249342746472E-3</v>
       </c>
+      <c r="CC14" s="1">
+        <v>8</v>
+      </c>
+      <c r="CD14" s="15">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="CE14" s="32">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="CF14" s="32">
+        <v>5.6030000000000003E-2</v>
+      </c>
+      <c r="CG14" s="32">
+        <v>5.8029999999999998E-2</v>
+      </c>
+      <c r="CH14" s="32">
+        <v>5.9000000000000004E-2</v>
+      </c>
+      <c r="CJ14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="CK14" s="18" cm="1">
+        <f t="array" ref="CK14">SUM((_xlfn.FLOOR.MATH(_xlfn.SEQUENCE($E$10*2-1)/($E$10*2-1))*100+$M$10*100)*(1+$CH$7:$CH$15/2)^-$CC$7:$CC$15)</f>
+        <v>96.216149644010343</v>
+      </c>
+      <c r="CL14" s="17">
+        <f t="shared" si="0"/>
+        <v>-3.7915333821010862E-3</v>
+      </c>
+      <c r="CN14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="CO14" s="17">
+        <v>-9.6211952963612644E-3</v>
+      </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.3">
       <c r="R15" s="19"/>
       <c r="S15" s="19"/>
       <c r="T15" s="19"/>
@@ -2993,8 +3456,40 @@
       <c r="AW15" s="17">
         <v>-4.3343850543170449E-2</v>
       </c>
+      <c r="CC15" s="1">
+        <v>9</v>
+      </c>
+      <c r="CD15" s="15">
+        <v>4.24E-2</v>
+      </c>
+      <c r="CE15" s="32">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="CF15" s="32">
+        <v>5.7270000000000001E-2</v>
+      </c>
+      <c r="CG15" s="32">
+        <v>5.9270000000000003E-2</v>
+      </c>
+      <c r="CH15" s="32">
+        <v>6.0299999999999999E-2</v>
+      </c>
+      <c r="CJ15" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="CL15" s="31">
+        <f>SUM(CL8:CL14)</f>
+        <v>-6.7670633004970143E-2</v>
+      </c>
+      <c r="CN15" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="CO15" s="44">
+        <f>SUM(_xlfn.ANCHORARRAY(CO16))</f>
+        <v>-1.1230886482698575E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
@@ -3077,8 +3572,31 @@
       <c r="AW16" s="17">
         <v>-5.4436272100378352E-2</v>
       </c>
+      <c r="CC16" s="1">
+        <v>10</v>
+      </c>
+      <c r="CD16" s="15">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="CE16" s="42"/>
+      <c r="CF16" s="42"/>
+      <c r="CG16" s="42"/>
+      <c r="CJ16" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="CL16" s="31">
+        <f>$M$10*100/CK7</f>
+        <v>2.4224866886810338E-2</v>
+      </c>
+      <c r="CN16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="CO16" s="17" cm="1">
+        <f t="array" ref="CO16:CO17">CL13:CL14</f>
+        <v>-7.4393531005974879E-3</v>
+      </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3156,9 +3674,36 @@
       <c r="AW17" s="31">
         <v>-4.8335440243914007E-2</v>
       </c>
+      <c r="CJ17" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="CL17" s="31">
+        <f>SUM(CL15:CL16)</f>
+        <v>-4.3445766118159805E-2</v>
+      </c>
+      <c r="CN17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="CO17" s="17">
+        <v>-3.7915333821010862E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:93" x14ac:dyDescent="0.3">
+      <c r="CN18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="CO18" s="31">
+        <f>SUM(CO7,CO11,CO15)</f>
+        <v>-4.3445766118159812E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="36">
+    <mergeCell ref="CC1:CW1"/>
+    <mergeCell ref="CD5:CH5"/>
+    <mergeCell ref="CN3:CO4"/>
+    <mergeCell ref="CJ3:CL4"/>
+    <mergeCell ref="CC3:CH3"/>
     <mergeCell ref="BS5:CA5"/>
     <mergeCell ref="BG5:BP5"/>
     <mergeCell ref="BR3:CA3"/>
@@ -3192,5 +3737,6 @@
     <mergeCell ref="W5:Y5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>